<commit_message>
PGD gen 2 seems to more or less be working
</commit_message>
<xml_diff>
--- a/Codi/PGD/data_100PQ.xlsx
+++ b/Codi/PGD/data_100PQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\Desktop\CITCEA\Codi\PGD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF55C19-2329-4791-911B-44554B2362F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4698307D-3C18-44C8-9E37-5D4E9C63C4C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43544277-89E4-4F72-87F2-FECA9F9384A7}"/>
   </bookViews>
@@ -533,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -557,7 +557,7 @@
       </c>
       <c r="B6">
         <f>B5</f>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:G21" si="0">C5</f>
@@ -586,7 +586,7 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:F70" si="1">B6</f>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -615,7 +615,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -644,7 +644,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -673,7 +673,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -731,7 +731,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -760,7 +760,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -789,7 +789,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -818,7 +818,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -847,7 +847,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -876,7 +876,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -905,7 +905,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -934,7 +934,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
@@ -963,7 +963,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
@@ -992,7 +992,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="B23">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B27">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="B28">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="B29">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B30">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="B31">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -1456,7 +1456,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
@@ -1862,7 +1862,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="B52">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B53">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="B54">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="B55">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="B56">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
@@ -2036,7 +2036,7 @@
       </c>
       <c r="B57">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B58">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B62">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
@@ -2210,7 +2210,7 @@
       </c>
       <c r="B63">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
@@ -2239,7 +2239,7 @@
       </c>
       <c r="B64">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="B65">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B66">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="B67">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="B68">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="B69">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="B71">
         <f t="shared" ref="B71:E104" si="4">B70</f>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C71">
         <f t="shared" si="4"/>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="B72">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C72">
         <f t="shared" si="4"/>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="B73">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C73">
         <f t="shared" si="4"/>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="B74">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C74">
         <f t="shared" si="4"/>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="B75">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C75">
         <f t="shared" si="4"/>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="B76">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C76">
         <f t="shared" si="4"/>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="B77">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C77">
         <f t="shared" si="4"/>
@@ -2645,7 +2645,7 @@
       </c>
       <c r="B78">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C78">
         <f t="shared" si="4"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="B79">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C79">
         <f t="shared" si="4"/>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="B80">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C80">
         <f t="shared" si="4"/>
@@ -2732,7 +2732,7 @@
       </c>
       <c r="B81">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C81">
         <f t="shared" si="4"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B82">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C82">
         <f t="shared" si="4"/>
@@ -2790,7 +2790,7 @@
       </c>
       <c r="B83">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C83">
         <f t="shared" si="4"/>
@@ -2819,7 +2819,7 @@
       </c>
       <c r="B84">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C84">
         <f t="shared" si="4"/>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B85">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C85">
         <f t="shared" si="4"/>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C86">
         <f t="shared" si="4"/>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="B87">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C87">
         <f t="shared" si="4"/>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="B88">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C88">
         <f t="shared" si="4"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="B89">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C89">
         <f t="shared" si="4"/>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="B90">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C90">
         <f t="shared" si="4"/>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="B91">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C91">
         <f t="shared" si="4"/>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="B92">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C92">
         <f t="shared" si="4"/>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="B93">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C93">
         <f t="shared" si="4"/>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="B94">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C94">
         <f t="shared" si="4"/>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="B95">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C95">
         <f t="shared" si="4"/>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="B96">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C96">
         <f t="shared" si="4"/>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="B97">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C97">
         <f t="shared" si="4"/>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="B98">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C98">
         <f t="shared" si="4"/>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="B99">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C99">
         <f t="shared" si="4"/>
@@ -3283,7 +3283,7 @@
       </c>
       <c r="B100">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C100">
         <f t="shared" si="4"/>
@@ -3312,7 +3312,7 @@
       </c>
       <c r="B101">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C101">
         <f t="shared" si="4"/>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B102">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C102">
         <f t="shared" si="4"/>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="B103">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C103">
         <f t="shared" si="4"/>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="B104">
         <f t="shared" si="4"/>
-        <v>-1E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="C104">
         <f t="shared" si="4"/>

</xml_diff>